<commit_message>
added create and remove operations to orders table
</commit_message>
<xml_diff>
--- a/docs/sample-database.xlsx
+++ b/docs/sample-database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suchi\OneDrive\Documents\Suchir\Programming-Projects\supply-chain-management-prototype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suchi\OneDrive\Documents\Suchir\Programming-Projects\supply-chain-management-prototype\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64769F26-9E96-4AAB-84D5-896BA8DB4F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBF3C38-2A96-47BF-9B7E-16589F05A712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D38B9A9A-713C-4E10-BD0E-D460C52D4172}"/>
   </bookViews>
@@ -144,9 +144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +514,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,7 +571,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -597,7 +600,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -626,7 +629,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -882,20 +885,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="65182052-a372-4731-a487-81ef5d44403b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="65182052-a372-4731-a487-81ef5d44403b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,14 +921,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B7C794A-CF2A-498F-A715-459E81BD4165}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9349DD7-A162-4A52-85D6-2B5E95B30209}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -940,4 +935,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B7C794A-CF2A-498F-A715-459E81BD4165}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>